<commit_message>
improved data output, test for failing r_hat OR peak criteria
</commit_message>
<xml_diff>
--- a/230418_Pipeline_test_Orn70/summary_peak_data.xlsx
+++ b/230418_Pipeline_test_Orn70/summary_peak_data.xlsx
@@ -524,7 +524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
commit Excel sheet changes to be able to create new branch
</commit_message>
<xml_diff>
--- a/230418_Pipeline_test_Orn70/summary_peak_data.xlsx
+++ b/230418_Pipeline_test_Orn70/summary_peak_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20985" windowHeight="10110"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20985" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,12 +525,13 @@
   <dimension ref="A1:M1281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>